<commit_message>
Vendor Document in UPPER case.
Vendor Document in UPPER case.
</commit_message>
<xml_diff>
--- a/App_Templates/QCL_Offered.xlsx
+++ b/App_Templates/QCL_Offered.xlsx
@@ -587,6 +587,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -605,13 +614,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -652,12 +658,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1021,89 +1021,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="35"/>
     </row>
     <row r="2" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="41"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="1:17" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="16"/>
     </row>
@@ -1134,27 +1134,27 @@
       <c r="P6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="28" t="s">
+      <c r="Q6" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="42" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="45" t="s">
@@ -1172,24 +1172,24 @@
       <c r="M7" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="28" t="s">
         <v>22</v>
       </c>
       <c r="P7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="29"/>
+      <c r="Q7" s="31"/>
     </row>
     <row r="8" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="44"/>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1207,10 +1207,10 @@
       </c>
       <c r="L8" s="52"/>
       <c r="M8" s="54"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
     </row>
   </sheetData>
   <sheetProtection password="CFCD" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
@@ -1232,14 +1232,14 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="P7:P8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Point 18, 17 and 18
</commit_message>
<xml_diff>
--- a/App_Templates/QCL_Offered.xlsx
+++ b/App_Templates/QCL_Offered.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\WebEitl1\App_Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5834A654-EE9D-47A2-ABD0-80AFA30457C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QC List" sheetId="1" r:id="rId1"/>
@@ -103,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,7 +548,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -573,10 +579,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,17 +587,59 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,12 +680,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -662,6 +700,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,71 +724,36 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -790,7 +802,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -823,9 +835,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -858,6 +887,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1033,7 +1079,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1058,113 +1104,113 @@
     <col min="14" max="14" width="8.140625" style="11" customWidth="1"/>
     <col min="15" max="15" width="7.85546875" style="11" customWidth="1"/>
     <col min="16" max="16" width="8" style="11" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" style="14" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" style="64" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" style="13" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="26"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="39"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="29"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="1:18" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="32"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="45"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
-      <c r="I4" s="54" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="I4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="61"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="58"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="17"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="I5" s="54" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="I5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="61"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="22"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="14"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
@@ -1173,87 +1219,87 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="39" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57" t="s">
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="41"/>
-      <c r="O6" s="18" t="s">
+      <c r="N6" s="55"/>
+      <c r="O6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="34" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="36" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="42" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="P7" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="46" t="s">
+      <c r="Q7" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="22"/>
+      <c r="R7" s="35"/>
     </row>
     <row r="8" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="34"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1269,28 +1315,17 @@
       <c r="L8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="43"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection password="CF0D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
-  <autoFilter ref="A8:R8"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SEmNNrPKhcRrFQqwWCmiYFIdZwCnPSxD0IZOr3V0mrw6NIThzTLXYSvfPOG70uMJOy3ME+aVccH2FQKHOP5Xmg==" saltValue="TC8RIJ/0R2WMErf3JkHJSg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
+  <autoFilter ref="A8:R8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="27">
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="R6:R8"/>
     <mergeCell ref="D1:R3"/>
@@ -1307,6 +1342,17 @@
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>